<commit_message>
fixed old order codes
</commit_message>
<xml_diff>
--- a/vbit3components.xlsx
+++ b/vbit3components.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="210" yWindow="495" windowWidth="18855" windowHeight="11445"/>
@@ -11,19 +11,16 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="101">
   <si>
     <t xml:space="preserve">  QTY=</t>
   </si>
   <si>
-    <t>VBIT-Pi  Kitting List</t>
-  </si>
-  <si>
     <t>Excess</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>PCB</t>
   </si>
   <si>
-    <t>VBIT</t>
-  </si>
-  <si>
     <t>0603 SM CAP</t>
   </si>
   <si>
@@ -96,9 +90,6 @@
     <t>390pF</t>
   </si>
   <si>
-    <t>0605</t>
-  </si>
-  <si>
     <t>C14</t>
   </si>
   <si>
@@ -138,9 +129,6 @@
     <t>Yellow</t>
   </si>
   <si>
-    <t>0805 SM INDUCTOR</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
@@ -159,9 +147,6 @@
     <t>P1</t>
   </si>
   <si>
-    <t>608-350</t>
-  </si>
-  <si>
     <t>P2 P3</t>
   </si>
   <si>
@@ -186,63 +171,42 @@
     <t>18R</t>
   </si>
   <si>
-    <t>9330747</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
     <t>56R</t>
   </si>
   <si>
-    <t>9332197</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
     <t>1k</t>
   </si>
   <si>
-    <t>9330380</t>
-  </si>
-  <si>
     <t>R4</t>
   </si>
   <si>
     <t>8R2</t>
   </si>
   <si>
-    <t>2141558</t>
-  </si>
-  <si>
     <t>R5</t>
   </si>
   <si>
     <t>47k</t>
   </si>
   <si>
-    <t>9331255</t>
-  </si>
-  <si>
     <t>R9</t>
   </si>
   <si>
     <t>220R</t>
   </si>
   <si>
-    <t>2008352</t>
-  </si>
-  <si>
     <t>SM IC SOT307-2 Video Processor</t>
   </si>
   <si>
     <t>U1</t>
   </si>
   <si>
-    <t>SAA7113H/V2</t>
-  </si>
-  <si>
     <t>TQFP44</t>
   </si>
   <si>
@@ -267,9 +231,6 @@
     <t>U3</t>
   </si>
   <si>
-    <t>SAA7121H</t>
-  </si>
-  <si>
     <t>SM IC Multiplexer</t>
   </si>
   <si>
@@ -303,12 +264,6 @@
     <t>HC49/S</t>
   </si>
   <si>
-    <t>DNF = Do Not Fit. AVR version only</t>
-  </si>
-  <si>
-    <t>Prototyping board</t>
-  </si>
-  <si>
     <t>Crystal</t>
   </si>
   <si>
@@ -337,6 +292,33 @@
   </si>
   <si>
     <t>Bin</t>
+  </si>
+  <si>
+    <t>SAA7113</t>
+  </si>
+  <si>
+    <t>SAA7121</t>
+  </si>
+  <si>
+    <t>* Depends on your crystal. Check it's datasheet</t>
+  </si>
+  <si>
+    <t>Information Correct as of 17/03/2019. Some of these components are now obsolete - don't worry, if they can't be found at Farnell they can be bought from UTSource.</t>
+  </si>
+  <si>
+    <t>Obsolete</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>VBIT-Pi 3 PCB</t>
+  </si>
+  <si>
+    <t>VBIT-Pi 3 Kitting List</t>
+  </si>
+  <si>
+    <t>PSG01547</t>
   </si>
 </sst>
 </file>
@@ -349,7 +331,7 @@
     <numFmt numFmtId="166" formatCode="&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="167" formatCode="[$£-809]#,##0.00;[Red]&quot;-&quot;[$£-809]#,##0.00"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,6 +393,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Arial1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -453,7 +441,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment horizontal="center"/>
@@ -464,8 +452,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -542,10 +534,21 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Heading" xfId="1"/>
     <cellStyle name="Heading1" xfId="2"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal_pb301bom" xfId="3"/>
     <cellStyle name="Result" xfId="4"/>
@@ -843,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV1048564"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1"/>
@@ -866,18 +869,20 @@
     <col min="257" max="1023" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="13.5" customHeight="1">
-      <c r="A1" s="7"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1"/>
+    <row r="1" spans="1:18" ht="14.25">
+      <c r="A1" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
       <c r="L1"/>
       <c r="M1"/>
       <c r="N1"/>
@@ -894,14 +899,14 @@
         <v>10</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -916,36 +921,38 @@
     </row>
     <row r="3" spans="1:18" s="2" customFormat="1" ht="28.5">
       <c r="A3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="D3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="E3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="G3" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="H3" s="15" t="s">
+      <c r="I3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3"/>
+      <c r="K3" s="14" t="s">
+        <v>96</v>
+      </c>
       <c r="L3"/>
       <c r="M3"/>
       <c r="N3"/>
@@ -956,13 +963,13 @@
     </row>
     <row r="4" spans="1:18" s="3" customFormat="1" ht="14.25">
       <c r="A4" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="7">
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -971,14 +978,14 @@
         <v>10</v>
       </c>
       <c r="G4" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H4" s="17">
         <f>SUM(G4-F4)</f>
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4"/>
@@ -992,36 +999,36 @@
     </row>
     <row r="5" spans="1:18" ht="14.25">
       <c r="A5" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="8">
         <v>10</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F5" s="16">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="G5" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="17">
         <f t="shared" ref="H5:H31" si="1">SUM(G5-F5)</f>
-        <v>-99</v>
+        <v>-100</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J5" s="9">
-        <v>1907036</v>
+        <v>317287</v>
       </c>
       <c r="K5"/>
       <c r="L5"/>
@@ -1034,36 +1041,36 @@
     </row>
     <row r="6" spans="1:18" ht="14.25">
       <c r="A6" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="8">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F6" s="16">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="G6" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H6" s="17">
         <f t="shared" si="1"/>
-        <v>-25</v>
+        <v>-30</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J6" s="7">
-        <v>8820007</v>
+        <v>1759116</v>
       </c>
       <c r="K6"/>
       <c r="L6"/>
@@ -1076,36 +1083,36 @@
     </row>
     <row r="7" spans="1:18" ht="14.25">
       <c r="A7" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="8">
         <v>1</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F7" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G7" s="7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H7" s="17">
         <f t="shared" si="1"/>
-        <v>-6</v>
+        <v>-10</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J7" s="18">
-        <v>1414606</v>
+        <v>1759088</v>
       </c>
       <c r="K7"/>
       <c r="L7"/>
@@ -1118,19 +1125,19 @@
     </row>
     <row r="8" spans="1:18" ht="14.25">
       <c r="A8" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="8">
         <v>2</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F8" s="16">
         <f t="shared" si="0"/>
@@ -1144,10 +1151,10 @@
         <v>-20</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J8" s="18">
-        <v>1865475</v>
+        <v>1759056</v>
       </c>
       <c r="K8"/>
       <c r="L8"/>
@@ -1160,36 +1167,36 @@
     </row>
     <row r="9" spans="1:18" ht="14.25">
       <c r="A9" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="8">
         <v>1</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>14</v>
       </c>
       <c r="F9" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G9" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H9" s="17">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J9" s="19">
-        <v>1414638</v>
+        <v>1759077</v>
       </c>
       <c r="K9"/>
       <c r="L9"/>
@@ -1202,36 +1209,36 @@
     </row>
     <row r="10" spans="1:18" ht="14.25">
       <c r="A10" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="8">
         <v>1</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F10" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G10" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H10" s="17">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J10" s="18">
-        <v>1414613</v>
+        <v>1759067</v>
       </c>
       <c r="K10"/>
       <c r="L10"/>
@@ -1244,36 +1251,36 @@
     </row>
     <row r="11" spans="1:18" ht="14.25">
       <c r="A11" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" s="8">
         <v>1</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F11" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G11" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H11" s="17">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J11" s="19">
-        <v>1828912</v>
+        <v>1759081</v>
       </c>
       <c r="K11"/>
       <c r="L11"/>
@@ -1286,19 +1293,19 @@
     </row>
     <row r="12" spans="1:18" ht="14.25">
       <c r="A12" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B12" s="8">
         <v>2</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="8">
-        <v>603</v>
+        <v>30</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>14</v>
       </c>
       <c r="F12" s="16">
         <f t="shared" si="0"/>
@@ -1312,10 +1319,10 @@
         <v>-20</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J12" s="18">
-        <v>9227830</v>
+        <v>2320817</v>
       </c>
       <c r="K12"/>
       <c r="L12"/>
@@ -1328,36 +1335,36 @@
     </row>
     <row r="13" spans="1:18" ht="14.25">
       <c r="A13" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="8">
         <v>1</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F13" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G13" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H13" s="17">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J13" s="22">
-        <v>2070396</v>
+        <v>2320755</v>
       </c>
       <c r="K13"/>
       <c r="L13"/>
@@ -1370,33 +1377,33 @@
     </row>
     <row r="14" spans="1:18" ht="14.25">
       <c r="A14" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B14" s="8">
         <v>1</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F14" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G14" s="7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H14" s="17">
         <f t="shared" si="1"/>
-        <v>-6</v>
+        <v>-10</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J14" s="21">
         <v>2099242</v>
@@ -1412,36 +1419,36 @@
     </row>
     <row r="15" spans="1:18" ht="14.25">
       <c r="A15" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="8">
         <v>1</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>34</v>
+        <v>38</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>14</v>
       </c>
       <c r="F15" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G15" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H15" s="17">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J15" s="9">
-        <v>2112892</v>
+        <v>2215635</v>
       </c>
       <c r="K15"/>
       <c r="L15"/>
@@ -1454,19 +1461,19 @@
     </row>
     <row r="16" spans="1:18" s="3" customFormat="1" ht="14.25">
       <c r="A16" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B16" s="8">
         <v>2</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F16" s="16">
         <f t="shared" si="0"/>
@@ -1480,7 +1487,7 @@
         <v>-20</v>
       </c>
       <c r="I16" s="20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J16" s="20">
         <v>1669530</v>
@@ -1496,19 +1503,19 @@
     </row>
     <row r="17" spans="1:256" ht="14.25">
       <c r="A17" s="8" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B17" s="8">
         <v>1</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="F17" s="16">
         <f t="shared" si="0"/>
@@ -1522,10 +1529,10 @@
         <v>-10</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J17" s="21" t="s">
-        <v>47</v>
+        <v>15</v>
+      </c>
+      <c r="J17" s="21">
+        <v>2847248</v>
       </c>
       <c r="K17"/>
       <c r="L17"/>
@@ -1538,17 +1545,19 @@
     </row>
     <row r="18" spans="1:256" ht="14.25">
       <c r="A18" s="8" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B18" s="8">
         <v>2</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="8"/>
+        <v>43</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="E18" s="8" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="F18" s="16">
         <f t="shared" si="0"/>
@@ -1562,7 +1571,10 @@
         <v>-20</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="J18" s="21">
+        <v>1280702</v>
       </c>
       <c r="K18"/>
       <c r="L18"/>
@@ -1575,33 +1587,33 @@
     </row>
     <row r="19" spans="1:256" ht="14.25">
       <c r="A19" s="8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B19" s="8">
         <v>1</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F19" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G19" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H19" s="17">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J19" s="23">
         <v>8737274</v>
@@ -1617,36 +1629,36 @@
     </row>
     <row r="20" spans="1:256" ht="14.25">
       <c r="A20" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B20" s="8">
         <v>1</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F20" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G20" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H20" s="17">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J20" s="21" t="s">
-        <v>56</v>
+        <v>15</v>
+      </c>
+      <c r="J20" s="26">
+        <v>2447270</v>
       </c>
       <c r="K20"/>
       <c r="L20"/>
@@ -1659,36 +1671,36 @@
     </row>
     <row r="21" spans="1:256" ht="14.25">
       <c r="A21" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B21" s="8">
         <v>1</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F21" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G21" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H21" s="17">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J21" s="21" t="s">
-        <v>59</v>
+        <v>15</v>
+      </c>
+      <c r="J21" s="26">
+        <v>2074286</v>
       </c>
       <c r="K21"/>
       <c r="L21"/>
@@ -1701,36 +1713,36 @@
     </row>
     <row r="22" spans="1:256" ht="14.25">
       <c r="A22" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B22" s="8">
         <v>1</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F22" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G22" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H22" s="17">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J22" s="21" t="s">
-        <v>62</v>
+        <v>15</v>
+      </c>
+      <c r="J22" s="26">
+        <v>2073354</v>
       </c>
       <c r="K22"/>
       <c r="L22"/>
@@ -1743,36 +1755,36 @@
     </row>
     <row r="23" spans="1:256" ht="14.25">
       <c r="A23" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B23" s="8">
         <v>1</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F23" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G23" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H23" s="17">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J23" s="21" t="s">
-        <v>65</v>
+        <v>15</v>
+      </c>
+      <c r="J23" s="26">
+        <v>2845969</v>
       </c>
       <c r="K23"/>
       <c r="L23"/>
@@ -1785,36 +1797,36 @@
     </row>
     <row r="24" spans="1:256" ht="14.25">
       <c r="A24" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B24" s="8">
         <v>1</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F24" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G24" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H24" s="17">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J24" s="21" t="s">
-        <v>68</v>
+        <v>15</v>
+      </c>
+      <c r="J24" s="26">
+        <v>2073510</v>
       </c>
       <c r="K24"/>
       <c r="L24"/>
@@ -1827,36 +1839,36 @@
     </row>
     <row r="25" spans="1:256" ht="14.25">
       <c r="A25" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B25" s="8">
         <v>1</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F25" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G25" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H25" s="17">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J25" s="21" t="s">
-        <v>71</v>
+        <v>15</v>
+      </c>
+      <c r="J25" s="26">
+        <v>2447298</v>
       </c>
       <c r="K25"/>
       <c r="L25"/>
@@ -1869,35 +1881,37 @@
     </row>
     <row r="26" spans="1:256" ht="14.25">
       <c r="A26" s="8" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B26" s="8">
         <v>1</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="F26" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G26" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H26" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="K26"/>
+        <v>64</v>
+      </c>
+      <c r="K26" t="s">
+        <v>97</v>
+      </c>
       <c r="L26"/>
       <c r="M26"/>
       <c r="N26"/>
@@ -1908,38 +1922,37 @@
     </row>
     <row r="27" spans="1:256" ht="14.25">
       <c r="A27" s="8" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B27" s="8">
         <v>1</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="F27" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G27" s="7">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="H27" s="17">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J27" s="21">
-        <v>9388338</v>
-      </c>
-      <c r="K27"/>
+        <v>64</v>
+      </c>
+      <c r="K27" t="s">
+        <v>97</v>
+      </c>
       <c r="L27"/>
       <c r="M27"/>
       <c r="N27"/>
@@ -1950,36 +1963,38 @@
     </row>
     <row r="28" spans="1:256" ht="14.25">
       <c r="A28" s="8" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B28" s="8">
         <v>1</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="F28" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G28" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H28" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="I28" s="19" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="J28" s="19"/>
-      <c r="K28"/>
+      <c r="K28" t="s">
+        <v>97</v>
+      </c>
       <c r="L28"/>
       <c r="M28"/>
       <c r="N28"/>
@@ -1990,19 +2005,19 @@
     </row>
     <row r="29" spans="1:256" ht="14.25">
       <c r="A29" s="8" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B29" s="8">
         <v>1</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="F29" s="16">
         <f t="shared" si="0"/>
@@ -2016,12 +2031,14 @@
         <v>-10</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J29" s="20">
         <v>1103068</v>
       </c>
-      <c r="K29"/>
+      <c r="K29" t="s">
+        <v>97</v>
+      </c>
       <c r="L29"/>
       <c r="M29"/>
       <c r="N29"/>
@@ -2032,19 +2049,19 @@
     </row>
     <row r="30" spans="1:256" ht="14.25">
       <c r="A30" s="8" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B30" s="8">
         <v>1</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="F30" s="16">
         <f t="shared" si="0"/>
@@ -2058,7 +2075,7 @@
         <v>-10</v>
       </c>
       <c r="I30" s="21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J30" s="21">
         <v>1695547</v>
@@ -2074,19 +2091,19 @@
     </row>
     <row r="31" spans="1:256" ht="14.25">
       <c r="A31" s="8" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B31" s="8">
         <v>1</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="F31" s="16">
         <f t="shared" si="0"/>
@@ -2100,7 +2117,7 @@
         <v>-10</v>
       </c>
       <c r="I31" s="18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J31" s="21">
         <v>1611790</v>
@@ -2135,11 +2152,11 @@
       <c r="IV32"/>
     </row>
     <row r="33" spans="1:256" ht="12.75" customHeight="1">
-      <c r="A33" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
+      <c r="A33" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="18"/>
@@ -2157,24 +2174,16 @@
       <c r="IV33"/>
     </row>
     <row r="34" spans="1:256" ht="14.25">
-      <c r="A34" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B34" s="8">
-        <v>1</v>
-      </c>
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
       <c r="H34" s="16"/>
-      <c r="I34" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="J34" s="24">
-        <v>2295747</v>
-      </c>
+      <c r="I34" s="18"/>
+      <c r="J34" s="24"/>
       <c r="K34"/>
       <c r="L34"/>
       <c r="M34"/>
@@ -2726,13 +2735,17 @@
       <c r="L1048564" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A33:C33"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J20" r:id="rId1"/>
-    <hyperlink ref="J21" r:id="rId2"/>
-    <hyperlink ref="J22" r:id="rId3"/>
-    <hyperlink ref="J23" r:id="rId4"/>
-    <hyperlink ref="J24" r:id="rId5"/>
-    <hyperlink ref="J25" r:id="rId6"/>
+    <hyperlink ref="J20" r:id="rId1" tooltip="2447270" display="https://uk.farnell.com/multicomp/mcwr06x18r0ftl/res-18r-1-0-1w-thick-film/dp/2447270?st=18r%200603"/>
+    <hyperlink ref="J21" r:id="rId2" tooltip="2074286" display="https://uk.farnell.com/multicomp/mcsr06x56r0ftl/res-56r-1-0-1w-0603-ceramic/dp/2074286?st=56r%200603%20multicomp"/>
+    <hyperlink ref="J22" r:id="rId3" tooltip="2073354" display="https://uk.farnell.com/multicomp/mcmr06x102-jtl/res-1k-5-0-1w-0603-ceramic/dp/2073354?st=1k%200603%20multicomp"/>
+    <hyperlink ref="J23" r:id="rId4" tooltip="2845969" display="https://uk.farnell.com/multicomp/mc0100w060318r20/res-8r2-1-0-1w-0603-thick-film/dp/2845969?st=8r2%200603%20multicomp"/>
+    <hyperlink ref="J24" r:id="rId5" tooltip="2073510" display="https://uk.farnell.com/multicomp/mcmr06x4702ftl/res-47k-1-0-1w-0603-ceramic/dp/2073510?st=47k%200603%20multicomp"/>
+    <hyperlink ref="J25" r:id="rId6" tooltip="2447298" display="https://uk.farnell.com/multicomp/mcwr06x2200ftl/res-220r-1-0-1w-0603-thick-film/dp/2447298?st=220r%200603%20multicomp"/>
   </hyperlinks>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="1.299212598425197" bottom="1.299212598425197" header="0.98425196850393704" footer="0.98425196850393704"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId7"/>

</xml_diff>

<commit_message>
Made some design for manufacturability layout improvements, changed some footprints and updated BOM
</commit_message>
<xml_diff>
--- a/vbit3components.xlsx
+++ b/vbit3components.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Documents\Projects\VBIT-Pi\vbit-pi-nathan\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="210" yWindow="495" windowWidth="18855" windowHeight="11445"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -324,14 +329,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0;[Red]&quot;-&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00&quot; &quot;;&quot;(£&quot;#,##0.00&quot;)&quot;"/>
     <numFmt numFmtId="166" formatCode="&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="167" formatCode="[$£-809]#,##0.00;[Red]&quot;-&quot;[$£-809]#,##0.00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,13 +404,49 @@
       <color theme="10"/>
       <name val="Arial1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -441,7 +482,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment horizontal="center"/>
@@ -456,8 +497,11 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -544,11 +588,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="9" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="10">
+    <cellStyle name="Bad" xfId="8" builtinId="27"/>
+    <cellStyle name="Good" xfId="7" builtinId="26"/>
     <cellStyle name="Heading" xfId="1"/>
     <cellStyle name="Heading1" xfId="2"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal_pb301bom" xfId="3"/>
     <cellStyle name="Result" xfId="4"/>
@@ -556,6 +612,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -602,7 +666,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -634,9 +698,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -668,6 +733,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -843,11 +909,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV1048564"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1"/>
@@ -997,7 +1063,7 @@
       <c r="Q4"/>
       <c r="R4"/>
     </row>
-    <row r="5" spans="1:18" ht="14.25">
+    <row r="5" spans="1:18" ht="15">
       <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
@@ -1007,7 +1073,7 @@
       <c r="C5" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="29" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="8" t="s">
@@ -1039,7 +1105,7 @@
       <c r="Q5"/>
       <c r="R5"/>
     </row>
-    <row r="6" spans="1:18" ht="14.25">
+    <row r="6" spans="1:18" ht="15">
       <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
@@ -1049,7 +1115,7 @@
       <c r="C6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="29" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="8" t="s">
@@ -1081,7 +1147,7 @@
       <c r="Q6"/>
       <c r="R6"/>
     </row>
-    <row r="7" spans="1:18" ht="14.25">
+    <row r="7" spans="1:18" ht="15">
       <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
@@ -1091,7 +1157,7 @@
       <c r="C7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="29" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="8" t="s">
@@ -1123,7 +1189,7 @@
       <c r="Q7"/>
       <c r="R7"/>
     </row>
-    <row r="8" spans="1:18" ht="14.25">
+    <row r="8" spans="1:18" ht="15">
       <c r="A8" s="8" t="s">
         <v>20</v>
       </c>
@@ -1133,7 +1199,7 @@
       <c r="C8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="29" t="s">
         <v>90</v>
       </c>
       <c r="E8" s="8" t="s">
@@ -1165,7 +1231,7 @@
       <c r="Q8"/>
       <c r="R8"/>
     </row>
-    <row r="9" spans="1:18" ht="14.25">
+    <row r="9" spans="1:18" ht="15">
       <c r="A9" s="8" t="s">
         <v>12</v>
       </c>
@@ -1175,7 +1241,7 @@
       <c r="C9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="29" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="25" t="s">
@@ -1207,7 +1273,7 @@
       <c r="Q9"/>
       <c r="R9"/>
     </row>
-    <row r="10" spans="1:18" ht="14.25">
+    <row r="10" spans="1:18" ht="15">
       <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
@@ -1217,7 +1283,7 @@
       <c r="C10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="29" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="8" t="s">
@@ -1249,7 +1315,7 @@
       <c r="Q10"/>
       <c r="R10"/>
     </row>
-    <row r="11" spans="1:18" ht="14.25">
+    <row r="11" spans="1:18" ht="15">
       <c r="A11" s="8" t="s">
         <v>12</v>
       </c>
@@ -1259,7 +1325,7 @@
       <c r="C11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="29" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="8" t="s">
@@ -1291,7 +1357,7 @@
       <c r="Q11"/>
       <c r="R11"/>
     </row>
-    <row r="12" spans="1:18" ht="14.25">
+    <row r="12" spans="1:18" ht="15">
       <c r="A12" s="8" t="s">
         <v>28</v>
       </c>
@@ -1301,7 +1367,7 @@
       <c r="C12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="29" t="s">
         <v>30</v>
       </c>
       <c r="E12" s="25" t="s">
@@ -1333,7 +1399,7 @@
       <c r="Q12"/>
       <c r="R12"/>
     </row>
-    <row r="13" spans="1:18" ht="14.25">
+    <row r="13" spans="1:18" ht="15">
       <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
@@ -1343,7 +1409,7 @@
       <c r="C13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="30" t="s">
         <v>33</v>
       </c>
       <c r="E13" s="8" t="s">
@@ -1375,7 +1441,7 @@
       <c r="Q13"/>
       <c r="R13"/>
     </row>
-    <row r="14" spans="1:18" ht="14.25">
+    <row r="14" spans="1:18" ht="15">
       <c r="A14" s="8" t="s">
         <v>34</v>
       </c>
@@ -1385,7 +1451,7 @@
       <c r="C14" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="29" t="s">
         <v>36</v>
       </c>
       <c r="E14" s="8" t="s">
@@ -1417,7 +1483,7 @@
       <c r="Q14"/>
       <c r="R14"/>
     </row>
-    <row r="15" spans="1:18" ht="14.25">
+    <row r="15" spans="1:18" ht="15">
       <c r="A15" s="8" t="s">
         <v>39</v>
       </c>
@@ -1427,7 +1493,7 @@
       <c r="C15" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="29" t="s">
         <v>38</v>
       </c>
       <c r="E15" s="25" t="s">
@@ -1459,7 +1525,7 @@
       <c r="Q15"/>
       <c r="R15"/>
     </row>
-    <row r="16" spans="1:18" s="3" customFormat="1" ht="14.25">
+    <row r="16" spans="1:18" s="3" customFormat="1" ht="15">
       <c r="A16" s="8" t="s">
         <v>39</v>
       </c>
@@ -1469,7 +1535,7 @@
       <c r="C16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="29" t="s">
         <v>41</v>
       </c>
       <c r="E16" s="8" t="s">
@@ -1501,7 +1567,7 @@
       <c r="Q16"/>
       <c r="R16"/>
     </row>
-    <row r="17" spans="1:256" ht="14.25">
+    <row r="17" spans="1:256" ht="15">
       <c r="A17" s="8" t="s">
         <v>87</v>
       </c>
@@ -1511,7 +1577,7 @@
       <c r="C17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="31" t="s">
         <v>88</v>
       </c>
       <c r="E17" s="8" t="s">
@@ -1543,7 +1609,7 @@
       <c r="Q17"/>
       <c r="R17"/>
     </row>
-    <row r="18" spans="1:256" ht="14.25">
+    <row r="18" spans="1:256" ht="15">
       <c r="A18" s="8" t="s">
         <v>85</v>
       </c>
@@ -1553,7 +1619,7 @@
       <c r="C18" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="29" t="s">
         <v>100</v>
       </c>
       <c r="E18" s="8" t="s">
@@ -1585,7 +1651,7 @@
       <c r="Q18"/>
       <c r="R18"/>
     </row>
-    <row r="19" spans="1:256" ht="14.25">
+    <row r="19" spans="1:256" ht="15">
       <c r="A19" s="8" t="s">
         <v>44</v>
       </c>
@@ -1595,7 +1661,7 @@
       <c r="C19" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="31" t="s">
         <v>46</v>
       </c>
       <c r="E19" s="8" t="s">
@@ -1627,7 +1693,7 @@
       <c r="Q19"/>
       <c r="R19"/>
     </row>
-    <row r="20" spans="1:256" ht="14.25">
+    <row r="20" spans="1:256" ht="15">
       <c r="A20" s="8" t="s">
         <v>48</v>
       </c>
@@ -1637,7 +1703,7 @@
       <c r="C20" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="29" t="s">
         <v>50</v>
       </c>
       <c r="E20" s="8" t="s">
@@ -1669,7 +1735,7 @@
       <c r="Q20"/>
       <c r="R20"/>
     </row>
-    <row r="21" spans="1:256" ht="14.25">
+    <row r="21" spans="1:256" ht="15">
       <c r="A21" s="8" t="s">
         <v>48</v>
       </c>
@@ -1679,7 +1745,7 @@
       <c r="C21" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="29" t="s">
         <v>52</v>
       </c>
       <c r="E21" s="8" t="s">
@@ -1711,7 +1777,7 @@
       <c r="Q21"/>
       <c r="R21"/>
     </row>
-    <row r="22" spans="1:256" ht="14.25">
+    <row r="22" spans="1:256" ht="15">
       <c r="A22" s="8" t="s">
         <v>48</v>
       </c>
@@ -1721,7 +1787,7 @@
       <c r="C22" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="31" t="s">
         <v>54</v>
       </c>
       <c r="E22" s="8" t="s">
@@ -1753,7 +1819,7 @@
       <c r="Q22"/>
       <c r="R22"/>
     </row>
-    <row r="23" spans="1:256" ht="14.25">
+    <row r="23" spans="1:256" ht="15">
       <c r="A23" s="8" t="s">
         <v>48</v>
       </c>
@@ -1763,7 +1829,7 @@
       <c r="C23" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="29" t="s">
         <v>56</v>
       </c>
       <c r="E23" s="8" t="s">
@@ -1795,7 +1861,7 @@
       <c r="Q23"/>
       <c r="R23"/>
     </row>
-    <row r="24" spans="1:256" ht="14.25">
+    <row r="24" spans="1:256" ht="15">
       <c r="A24" s="8" t="s">
         <v>48</v>
       </c>
@@ -1805,7 +1871,7 @@
       <c r="C24" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="31" t="s">
         <v>58</v>
       </c>
       <c r="E24" s="8" t="s">
@@ -1837,7 +1903,7 @@
       <c r="Q24"/>
       <c r="R24"/>
     </row>
-    <row r="25" spans="1:256" ht="14.25">
+    <row r="25" spans="1:256" ht="15">
       <c r="A25" s="8" t="s">
         <v>48</v>
       </c>
@@ -1847,7 +1913,7 @@
       <c r="C25" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="29" t="s">
         <v>60</v>
       </c>
       <c r="E25" s="8" t="s">
@@ -1879,7 +1945,7 @@
       <c r="Q25"/>
       <c r="R25"/>
     </row>
-    <row r="26" spans="1:256" ht="14.25">
+    <row r="26" spans="1:256" ht="15">
       <c r="A26" s="8" t="s">
         <v>61</v>
       </c>
@@ -1889,7 +1955,7 @@
       <c r="C26" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="29" t="s">
         <v>92</v>
       </c>
       <c r="E26" s="8" t="s">
@@ -1920,7 +1986,7 @@
       <c r="Q26"/>
       <c r="R26"/>
     </row>
-    <row r="27" spans="1:256" ht="14.25">
+    <row r="27" spans="1:256" ht="15">
       <c r="A27" s="8" t="s">
         <v>65</v>
       </c>
@@ -1930,7 +1996,7 @@
       <c r="C27" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="29" t="s">
         <v>67</v>
       </c>
       <c r="E27" s="8" t="s">
@@ -1961,7 +2027,7 @@
       <c r="Q27"/>
       <c r="R27"/>
     </row>
-    <row r="28" spans="1:256" ht="14.25">
+    <row r="28" spans="1:256" ht="15">
       <c r="A28" s="8" t="s">
         <v>69</v>
       </c>
@@ -1971,7 +2037,7 @@
       <c r="C28" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="29" t="s">
         <v>93</v>
       </c>
       <c r="E28" s="8" t="s">
@@ -2003,7 +2069,7 @@
       <c r="Q28"/>
       <c r="R28"/>
     </row>
-    <row r="29" spans="1:256" ht="14.25">
+    <row r="29" spans="1:256" ht="15">
       <c r="A29" s="8" t="s">
         <v>71</v>
       </c>
@@ -2013,7 +2079,7 @@
       <c r="C29" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="29" t="s">
         <v>73</v>
       </c>
       <c r="E29" s="8" t="s">
@@ -2047,7 +2113,7 @@
       <c r="Q29"/>
       <c r="R29"/>
     </row>
-    <row r="30" spans="1:256" ht="14.25">
+    <row r="30" spans="1:256" ht="15">
       <c r="A30" s="8" t="s">
         <v>75</v>
       </c>
@@ -2057,7 +2123,7 @@
       <c r="C30" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="29" t="s">
         <v>77</v>
       </c>
       <c r="E30" s="8" t="s">
@@ -2089,7 +2155,7 @@
       <c r="Q30"/>
       <c r="R30"/>
     </row>
-    <row r="31" spans="1:256" ht="14.25">
+    <row r="31" spans="1:256" ht="15">
       <c r="A31" s="8" t="s">
         <v>82</v>
       </c>
@@ -2099,7 +2165,7 @@
       <c r="C31" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="29" t="s">
         <v>80</v>
       </c>
       <c r="E31" s="8" t="s">
@@ -2754,7 +2820,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2771,7 +2837,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>